<commit_message>
Enable RoboZonky to keep pre-set minimal balance
Closes #25.
</commit_message>
<xml_diff>
--- a/robozonky-strategy-rules/src/test/resources/com/github/triceo/robozonky/strategy/rules/ExampleStrategy.xlsx
+++ b/robozonky-strategy-rules/src/test/resources/com/github/triceo/robozonky/strategy/rules/ExampleStrategy.xlsx
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
   <si>
     <t xml:space="preserve">RuleSet</t>
   </si>
@@ -235,6 +235,9 @@
     <t xml:space="preserve">$l: ProposedLoan</t>
   </si>
   <si>
+    <t xml:space="preserve">AvailableBalance</t>
+  </si>
+  <si>
     <t xml:space="preserve">not AcceptedLoan(id == $l.getId());RatingShare</t>
   </si>
   <si>
@@ -247,6 +250,9 @@
     <t xml:space="preserve">termInMonths &gt; $1, termInMonths &lt;= $2</t>
   </si>
   <si>
+    <t xml:space="preserve">value &gt;= $1, value &lt;= $2</t>
+  </si>
+  <si>
     <t xml:space="preserve">rating == $l.rating, share &gt;= $1, share &lt;= $2</t>
   </si>
   <si>
@@ -265,6 +271,9 @@
     <t xml:space="preserve">Term is between</t>
   </si>
   <si>
+    <t xml:space="preserve">Available balance is between</t>
+  </si>
+  <si>
     <t xml:space="preserve">Current share of this rating is between</t>
   </si>
   <si>
@@ -346,9 +355,6 @@
     <t xml:space="preserve">RatingShare</t>
   </si>
   <si>
-    <t xml:space="preserve">AvailableBalance</t>
-  </si>
-  <si>
     <t xml:space="preserve">Id == $a.id, rating == Rating.$1</t>
   </si>
   <si>
@@ -356,9 +362,6 @@
   </si>
   <si>
     <t xml:space="preserve">modify ($a) { setAmount($1) }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available balance is between</t>
   </si>
   <si>
     <t xml:space="preserve">Do not change</t>
@@ -806,27 +809,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:25"/>
+  <dimension ref="A1:IW25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="9:9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="0.127551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.2959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.1530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.6938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.6173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="30.1122448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="21.2295918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.6377551020408"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.1734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="17.6479591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.3877551020408"/>
-    <col collapsed="false" hidden="false" max="256" min="12" style="1" width="9.62755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="9.13265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.0459183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.4438775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.2397959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="31.1020408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="21.8520408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.2602040816327"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.1428571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.8826530612245"/>
+    <col collapsed="false" hidden="false" max="257" min="13" style="1" width="9.87244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.37755102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -837,7 +840,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="0"/>
+      <c r="H1" s="3"/>
       <c r="I1" s="0"/>
       <c r="J1" s="0"/>
       <c r="K1" s="0"/>
@@ -1086,8 +1089,9 @@
       <c r="IT1" s="0"/>
       <c r="IU1" s="0"/>
       <c r="IV1" s="0"/>
+      <c r="IW1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="0"/>
       <c r="C2" s="4" t="s">
@@ -1098,11 +1102,11 @@
       </c>
       <c r="E2" s="0"/>
       <c r="F2" s="0"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="6"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="0"/>
+      <c r="K2" s="6"/>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
       <c r="N2" s="0"/>
@@ -1348,8 +1352,9 @@
       <c r="IT2" s="0"/>
       <c r="IU2" s="0"/>
       <c r="IV2" s="0"/>
+      <c r="IW2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="3" customFormat="false" ht="37" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A3" s="0"/>
       <c r="B3" s="0"/>
       <c r="C3" s="4" t="s">
@@ -1360,11 +1365,11 @@
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="6"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
-      <c r="K3" s="0"/>
+      <c r="K3" s="6"/>
       <c r="L3" s="0"/>
       <c r="M3" s="0"/>
       <c r="N3" s="0"/>
@@ -1610,8 +1615,9 @@
       <c r="IT3" s="0"/>
       <c r="IU3" s="0"/>
       <c r="IV3" s="0"/>
+      <c r="IW3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="4" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A4" s="0"/>
       <c r="B4" s="0"/>
       <c r="C4" s="4" t="s">
@@ -1622,12 +1628,12 @@
       </c>
       <c r="E4" s="0"/>
       <c r="F4" s="0"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="0"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="8"/>
+      <c r="G4" s="0"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="0"/>
+      <c r="J4" s="6"/>
       <c r="K4" s="8"/>
-      <c r="L4" s="0"/>
+      <c r="L4" s="8"/>
       <c r="M4" s="0"/>
       <c r="N4" s="0"/>
       <c r="O4" s="0"/>
@@ -1872,6 +1878,7 @@
       <c r="IT4" s="0"/>
       <c r="IU4" s="0"/>
       <c r="IV4" s="0"/>
+      <c r="IW4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
@@ -2130,8 +2137,9 @@
       <c r="IT5" s="0"/>
       <c r="IU5" s="0"/>
       <c r="IV5" s="0"/>
+      <c r="IW5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A6" s="0"/>
       <c r="B6" s="9"/>
       <c r="C6" s="10" t="s">
@@ -2141,7 +2149,7 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
-      <c r="H6" s="0"/>
+      <c r="H6" s="11"/>
       <c r="I6" s="0"/>
       <c r="J6" s="0"/>
       <c r="K6" s="0"/>
@@ -2390,8 +2398,9 @@
       <c r="IT6" s="0"/>
       <c r="IU6" s="0"/>
       <c r="IV6" s="0"/>
+      <c r="IW6" s="0"/>
     </row>
-    <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="7" s="1" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B7" s="12"/>
       <c r="C7" s="13" t="s">
         <v>7</v>
@@ -2406,11 +2415,13 @@
         <v>7</v>
       </c>
       <c r="G7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="AMJ7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A8" s="0"/>
       <c r="B8" s="12"/>
       <c r="C8" s="15" t="s">
@@ -2418,11 +2429,13 @@
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="0"/>
+      <c r="G8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="14"/>
       <c r="I8" s="0"/>
       <c r="J8" s="0"/>
       <c r="K8" s="0"/>
@@ -2671,47 +2684,52 @@
       <c r="IT8" s="0"/>
       <c r="IU8" s="0"/>
       <c r="IV8" s="0"/>
+      <c r="IW8" s="0"/>
     </row>
-    <row r="9" s="17" customFormat="true" ht="39" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="9" s="17" customFormat="true" ht="31.5" hidden="true" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B9" s="18"/>
       <c r="C9" s="19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="F9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="AMJ9" s="0"/>
+      <c r="G9" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="16.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
       <c r="B10" s="22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="0"/>
+        <v>22</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>24</v>
+      </c>
       <c r="I10" s="0"/>
       <c r="J10" s="0"/>
       <c r="K10" s="0"/>
@@ -2960,26 +2978,27 @@
       <c r="IT10" s="0"/>
       <c r="IU10" s="0"/>
       <c r="IV10" s="0"/>
+      <c r="IW10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
       <c r="B11" s="26" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="28" t="n">
+        <v>27</v>
+      </c>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="H11" s="0"/>
       <c r="I11" s="0"/>
       <c r="J11" s="0"/>
       <c r="K11" s="0"/>
@@ -3228,24 +3247,25 @@
       <c r="IT11" s="0"/>
       <c r="IU11" s="0"/>
       <c r="IV11" s="0"/>
+      <c r="IW11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0"/>
       <c r="B12" s="26"/>
       <c r="C12" s="27" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D12" s="28"/>
       <c r="E12" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="28" t="n">
+      <c r="F12" s="29"/>
+      <c r="G12" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="H12" s="0"/>
       <c r="I12" s="0"/>
       <c r="J12" s="0"/>
       <c r="K12" s="0"/>
@@ -3494,24 +3514,25 @@
       <c r="IT12" s="0"/>
       <c r="IU12" s="0"/>
       <c r="IV12" s="0"/>
+      <c r="IW12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
       <c r="B13" s="26"/>
       <c r="C13" s="27" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D13" s="28"/>
       <c r="E13" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="28" t="n">
+        <v>32</v>
+      </c>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="28" t="n">
         <v>3</v>
       </c>
-      <c r="H13" s="0"/>
       <c r="I13" s="0"/>
       <c r="J13" s="0"/>
       <c r="K13" s="0"/>
@@ -3760,26 +3781,27 @@
       <c r="IT13" s="0"/>
       <c r="IU13" s="0"/>
       <c r="IV13" s="0"/>
+      <c r="IW13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0"/>
       <c r="B14" s="26"/>
       <c r="C14" s="27" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="28" t="n">
+        <v>36</v>
+      </c>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="H14" s="0"/>
       <c r="I14" s="0"/>
       <c r="J14" s="0"/>
       <c r="K14" s="0"/>
@@ -4028,24 +4050,25 @@
       <c r="IT14" s="0"/>
       <c r="IU14" s="0"/>
       <c r="IV14" s="0"/>
+      <c r="IW14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0"/>
       <c r="B15" s="26"/>
       <c r="C15" s="27" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E15" s="29"/>
-      <c r="F15" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" s="28" t="n">
+      <c r="F15" s="29"/>
+      <c r="G15" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="H15" s="0"/>
       <c r="I15" s="0"/>
       <c r="J15" s="0"/>
       <c r="K15" s="0"/>
@@ -4294,24 +4317,25 @@
       <c r="IT15" s="0"/>
       <c r="IU15" s="0"/>
       <c r="IV15" s="0"/>
+      <c r="IW15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0"/>
       <c r="B16" s="26"/>
       <c r="C16" s="27" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E16" s="29"/>
-      <c r="F16" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="28" t="n">
+      <c r="F16" s="29"/>
+      <c r="G16" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="28" t="n">
         <v>6</v>
       </c>
-      <c r="H16" s="0"/>
       <c r="I16" s="0"/>
       <c r="J16" s="0"/>
       <c r="K16" s="0"/>
@@ -4560,24 +4584,25 @@
       <c r="IT16" s="0"/>
       <c r="IU16" s="0"/>
       <c r="IV16" s="0"/>
+      <c r="IW16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
       <c r="B17" s="26"/>
       <c r="C17" s="30" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E17" s="32"/>
-      <c r="F17" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="32" t="n">
+      <c r="F17" s="32"/>
+      <c r="G17" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="32" t="n">
         <v>7</v>
       </c>
-      <c r="H17" s="0"/>
       <c r="I17" s="0"/>
       <c r="J17" s="0"/>
       <c r="K17" s="0"/>
@@ -4826,6 +4851,7 @@
       <c r="IT17" s="0"/>
       <c r="IU17" s="0"/>
       <c r="IV17" s="0"/>
+      <c r="IW17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0"/>
@@ -5084,11 +5110,12 @@
       <c r="IT18" s="0"/>
       <c r="IU18" s="0"/>
       <c r="IV18" s="0"/>
+      <c r="IW18" s="0"/>
     </row>
-    <row r="19" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="19" s="1" customFormat="true" ht="12.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B19" s="9"/>
       <c r="C19" s="10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
@@ -5096,9 +5123,9 @@
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
-      <c r="AMJ19" s="0"/>
+      <c r="J19" s="0"/>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="20" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B20" s="12"/>
       <c r="C20" s="13" t="s">
         <v>7</v>
@@ -5116,115 +5143,121 @@
         <v>7</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I20" s="14" t="s">
         <v>8</v>
       </c>
+      <c r="J20" s="0"/>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="21" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B21" s="12"/>
       <c r="C21" s="15" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
-      <c r="F21" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>47</v>
+      <c r="F21" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
+      <c r="J21" s="0"/>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="22" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B22" s="18"/>
       <c r="C22" s="19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="20" t="s">
-        <v>49</v>
+      <c r="F22" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>16</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="20" t="s">
-        <v>50</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="J22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="22.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I23" s="25" t="s">
-        <v>53</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="J23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="19.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="28"/>
       <c r="H24" s="29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I24" s="29" t="n">
         <v>400</v>
       </c>
+      <c r="J24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="26"/>
       <c r="C25" s="30" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D25" s="31"/>
       <c r="E25" s="31"/>
       <c r="F25" s="31"/>
       <c r="G25" s="31"/>
       <c r="H25" s="31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I25" s="31" t="n">
         <v>200</v>
       </c>
+      <c r="J25" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="D3:G3"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="B11:B17"/>
     <mergeCell ref="C21:E21"/>

</xml_diff>

<commit_message>
RoboZonky gets a public API module
</commit_message>
<xml_diff>
--- a/robozonky-strategy-rules/src/test/resources/com/github/triceo/robozonky/strategy/rules/ExampleStrategy.xlsx
+++ b/robozonky-strategy-rules/src/test/resources/com/github/triceo/robozonky/strategy/rules/ExampleStrategy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" state="visible" r:id="rId2"/>
@@ -214,7 +214,7 @@
     <t xml:space="preserve">Import</t>
   </si>
   <si>
-    <t xml:space="preserve">com.github.triceo.robozonky.remote.Rating, com.github.triceo.robozonky.strategy.rules.facts.ProposedLoan, com.github.triceo.robozonky.strategy.rules.facts.AcceptedLoan, com.github.triceo.robozonky.strategy.rules.facts.RatingShare, com.github.triceo.robozonky.strategy.rules.facts.Wallet</t>
+    <t xml:space="preserve">com.github.triceo.robozonky.api.remote.entities.Rating, com.github.triceo.robozonky.strategy.rules.facts.ProposedLoan, com.github.triceo.robozonky.strategy.rules.facts.AcceptedLoan, com.github.triceo.robozonky.strategy.rules.facts.RatingShare, com.github.triceo.robozonky.strategy.rules.facts.Wallet</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -809,24 +809,24 @@
   <dimension ref="A1:IW25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="0.127551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.780612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.1428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.2959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.8622448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="32.0918367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.5867346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.8724489795918"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="17.1530612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.6377551020408"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="19.5"/>
-    <col collapsed="false" hidden="false" max="257" min="13" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.62755102040816"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="0.13265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="257" min="13" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.44897959183673"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5262,7 +5262,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.15" right="0.140277777777778" top="0.179861111111111" bottom="0.2" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Move enums into their own package
After this is done, this package suddenly stops passing on mutation coverage, which is why we're introducing test coverage for enum Deserialization.
</commit_message>
<xml_diff>
--- a/robozonky-strategy-rules/src/test/resources/com/github/triceo/robozonky/strategy/rules/ExampleStrategy.xlsx
+++ b/robozonky-strategy-rules/src/test/resources/com/github/triceo/robozonky/strategy/rules/ExampleStrategy.xlsx
@@ -214,7 +214,7 @@
     <t xml:space="preserve">Import</t>
   </si>
   <si>
-    <t xml:space="preserve">com.github.triceo.robozonky.api.remote.entities.Rating, com.github.triceo.robozonky.strategy.rules.facts.ProposedLoan, com.github.triceo.robozonky.strategy.rules.facts.AcceptedLoan, com.github.triceo.robozonky.strategy.rules.facts.RatingShare, com.github.triceo.robozonky.strategy.rules.facts.Wallet</t>
+    <t xml:space="preserve">com.github.triceo.robozonky.api.remote.enums.Rating, com.github.triceo.robozonky.strategy.rules.facts.ProposedLoan, com.github.triceo.robozonky.strategy.rules.facts.AcceptedLoan, com.github.triceo.robozonky.strategy.rules.facts.RatingShare, com.github.triceo.robozonky.strategy.rules.facts.Wallet</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -809,24 +809,24 @@
   <dimension ref="A1:IW25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="0.13265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="257" min="13" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="257" min="13" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.17857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>